<commit_message>
add a legend to pie chart
</commit_message>
<xml_diff>
--- a/housing_list.xlsx
+++ b/housing_list.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C367"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,10 +399,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1300</v>
+        <v>800</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -410,13 +410,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -432,10 +432,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="B5">
-        <v>20223</v>
+        <v>1</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -443,32 +443,32 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>800</v>
+        <v>2878</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>650</v>
+        <v>566</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -476,10 +476,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>550</v>
+        <v>650</v>
       </c>
       <c r="B9">
-        <v>271</v>
+        <v>1</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -493,23 +493,23 @@
         <v>1</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>800</v>
+        <v>200</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1080</v>
+        <v>635</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -520,29 +520,29 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>420</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>550</v>
+        <v>900</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -553,18 +553,18 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>650</v>
+        <v>1</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>550</v>
+        <v>350</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -575,18 +575,18 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>1595</v>
+        <v>1</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -597,29 +597,29 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>765</v>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>950</v>
+        <v>1250</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>700</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>1300</v>
+        <v>1050</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -641,18 +641,18 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>1</v>
+        <v>675</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -663,10 +663,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>2000</v>
+        <v>730</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -674,7 +674,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>1</v>
+        <v>650</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>850</v>
+        <v>1</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>750</v>
+        <v>1</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -707,29 +707,29 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>1000</v>
+        <v>780</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>1</v>
+        <v>1250</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>575</v>
+        <v>1</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -740,18 +740,18 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>650</v>
+        <v>750</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -773,13 +773,13 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>1200</v>
+        <v>1700</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -795,29 +795,29 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>999</v>
+        <v>900</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>1200</v>
+        <v>750</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -828,18 +828,18 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -883,10 +883,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
@@ -894,18 +894,18 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -927,10 +927,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>350</v>
+        <v>1</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -938,29 +938,29 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>400</v>
+        <v>950</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>150</v>
+        <v>1500</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>650</v>
+        <v>1000</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -971,21 +971,21 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>850</v>
+        <v>700</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>550</v>
+        <v>900</v>
       </c>
       <c r="B55">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>1950</v>
+        <v>0</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1004,29 +1004,29 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>925</v>
+        <v>1</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>1168</v>
+        <v>1</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1040,7 +1040,7 @@
         <v>800</v>
       </c>
       <c r="B60">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>
@@ -1048,18 +1048,18 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>1412</v>
+        <v>600</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>1150</v>
+        <v>1</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -1070,29 +1070,29 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>1200</v>
+        <v>1</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>1</v>
+        <v>850</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -1103,18 +1103,18 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>2400</v>
+        <v>1050</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>1</v>
+        <v>1200</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>700</v>
+        <v>750</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>1</v>
+        <v>750</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -1202,10 +1202,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>1400</v>
+        <v>1950</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -1213,29 +1213,29 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>900</v>
+        <v>568</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -1246,32 +1246,32 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>1200</v>
+        <v>1</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>950</v>
+        <v>1</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>20223</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -1279,10 +1279,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>879</v>
+        <v>1595</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
@@ -1290,18 +1290,18 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>271</v>
       </c>
       <c r="C83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>795</v>
+        <v>765</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -1312,10 +1312,10 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>500</v>
+        <v>610</v>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>300</v>
+        <v>1300</v>
       </c>
       <c r="B86">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -1334,18 +1334,18 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>1050</v>
+        <v>1000</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>1</v>
+        <v>1200</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -1356,32 +1356,32 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>1</v>
+        <v>1300</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>1750</v>
+        <v>700</v>
       </c>
       <c r="B90">
         <v>1</v>
       </c>
       <c r="C90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>700</v>
+        <v>965</v>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C91" t="b">
         <v>0</v>
@@ -1389,21 +1389,21 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>950</v>
+        <v>570</v>
       </c>
       <c r="B92">
         <v>1</v>
       </c>
       <c r="C92" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>650</v>
+        <v>1300</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C93" t="b">
         <v>1</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>999</v>
+        <v>800</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C96" t="b">
         <v>1</v>
@@ -1455,32 +1455,32 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>2500</v>
+        <v>1</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
       <c r="C98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>800</v>
+        <v>150</v>
       </c>
       <c r="B99">
         <v>1</v>
       </c>
       <c r="C99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>900</v>
+        <v>1</v>
       </c>
       <c r="B100">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C100" t="b">
         <v>1</v>
@@ -1488,10 +1488,10 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="B101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C101" t="b">
         <v>1</v>
@@ -1499,18 +1499,18 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="B102">
         <v>1</v>
       </c>
       <c r="C102" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104">
-        <v>800</v>
+        <v>999</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106">
-        <v>1</v>
+        <v>999</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -1565,24 +1565,24 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
       <c r="C108" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C109" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1598,18 +1598,18 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111">
-        <v>1</v>
+        <v>750</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
       <c r="C111" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112">
-        <v>800</v>
+        <v>1</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -1620,10 +1620,10 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C113" t="b">
         <v>1</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115">
-        <v>1</v>
+        <v>650</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -1675,18 +1675,18 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118">
-        <v>375</v>
+        <v>1</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
       <c r="C118" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119">
-        <v>650</v>
+        <v>1</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121">
-        <v>1200</v>
+        <v>600</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -1719,7 +1719,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -1741,21 +1741,21 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124">
-        <v>825</v>
+        <v>800</v>
       </c>
       <c r="B124">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C124" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125">
-        <v>700</v>
+        <v>1</v>
       </c>
       <c r="B125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C125" t="b">
         <v>1</v>
@@ -1763,21 +1763,21 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="B126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C126" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127">
-        <v>850</v>
+        <v>1</v>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C127" t="b">
         <v>1</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="128" spans="1:3">
       <c r="A128">
-        <v>300</v>
+        <v>800</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -1796,10 +1796,10 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129">
-        <v>850</v>
+        <v>1000</v>
       </c>
       <c r="B129">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C129" t="b">
         <v>1</v>
@@ -1810,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="B130">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C130" t="b">
         <v>1</v>
@@ -1818,13 +1818,13 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="B131">
         <v>1</v>
       </c>
       <c r="C131" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1840,7 +1840,7 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -1851,10 +1851,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C134" t="b">
         <v>1</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135">
-        <v>750</v>
+        <v>1</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136">
-        <v>800</v>
+        <v>1</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -1906,29 +1906,29 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140">
-        <v>1</v>
+        <v>2600</v>
       </c>
       <c r="B140">
         <v>1</v>
       </c>
       <c r="C140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141">
-        <v>123456</v>
+        <v>1</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -1945,12 +1945,12 @@
         <v>1</v>
       </c>
       <c r="C142" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143">
-        <v>750</v>
+        <v>650</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -1961,7 +1961,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -1972,18 +1972,18 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145">
-        <v>800</v>
+        <v>49</v>
       </c>
       <c r="B145">
         <v>1</v>
       </c>
       <c r="C145" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146">
-        <v>2000</v>
+        <v>123456</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -1994,13 +1994,13 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147">
-        <v>1</v>
+        <v>650</v>
       </c>
       <c r="B147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C147" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2016,7 +2016,7 @@
     </row>
     <row r="149" spans="1:3">
       <c r="A149">
-        <v>800</v>
+        <v>1</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -2027,10 +2027,10 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="B150">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C150" t="b">
         <v>0</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -2049,29 +2049,29 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="B152">
         <v>1</v>
       </c>
       <c r="C152" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153">
-        <v>1</v>
+        <v>950</v>
       </c>
       <c r="B153">
         <v>1</v>
       </c>
       <c r="C153" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="B154">
         <v>1</v>
@@ -2082,7 +2082,7 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155">
-        <v>1300</v>
+        <v>1</v>
       </c>
       <c r="B155">
         <v>1</v>
@@ -2093,21 +2093,21 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="B156">
         <v>1</v>
       </c>
       <c r="C156" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="B157">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C157" t="b">
         <v>1</v>
@@ -2115,13 +2115,13 @@
     </row>
     <row r="158" spans="1:3">
       <c r="A158">
-        <v>800</v>
+        <v>1</v>
       </c>
       <c r="B158">
         <v>1</v>
       </c>
       <c r="C158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2129,10 +2129,10 @@
         <v>1</v>
       </c>
       <c r="B159">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C159" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2140,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C160" t="b">
         <v>1</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -2159,10 +2159,10 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162">
-        <v>750</v>
+        <v>1200</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C162" t="b">
         <v>1</v>
@@ -2170,24 +2170,24 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B163">
         <v>1</v>
       </c>
       <c r="C163" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="B164">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C164" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2198,12 +2198,12 @@
         <v>1</v>
       </c>
       <c r="C165" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -2225,21 +2225,21 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="B168">
         <v>1</v>
       </c>
       <c r="C168" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="B169">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C169" t="b">
         <v>0</v>
@@ -2247,10 +2247,10 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="B170">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C170" t="b">
         <v>1</v>
@@ -2258,18 +2258,18 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171">
-        <v>1200</v>
+        <v>925</v>
       </c>
       <c r="B171">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C171" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172">
-        <v>700</v>
+        <v>750</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -2280,18 +2280,18 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="B173">
         <v>1</v>
       </c>
       <c r="C173" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174">
-        <v>1</v>
+        <v>1150</v>
       </c>
       <c r="B174">
         <v>1</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -2313,10 +2313,10 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="B176">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C176" t="b">
         <v>1</v>
@@ -2324,18 +2324,18 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="B177">
         <v>1</v>
       </c>
       <c r="C177" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -2346,21 +2346,21 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B179">
         <v>1</v>
       </c>
       <c r="C179" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B180">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C180" t="b">
         <v>1</v>
@@ -2368,10 +2368,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B181">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C181" t="b">
         <v>1</v>
@@ -2379,10 +2379,10 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182">
-        <v>0</v>
+        <v>879</v>
       </c>
       <c r="B182">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C182" t="b">
         <v>0</v>
@@ -2401,7 +2401,7 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184">
-        <v>1</v>
+        <v>850</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -2415,15 +2415,15 @@
         <v>1300</v>
       </c>
       <c r="B185">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C185" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186">
-        <v>750</v>
+        <v>375</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -2434,10 +2434,10 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187">
-        <v>800</v>
+        <v>1</v>
       </c>
       <c r="B187">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C187" t="b">
         <v>1</v>
@@ -2445,13 +2445,13 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="B188">
-        <v>20223</v>
+        <v>1</v>
       </c>
       <c r="C188" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2467,7 +2467,7 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190">
-        <v>650</v>
+        <v>1412</v>
       </c>
       <c r="B190">
         <v>1</v>
@@ -2481,7 +2481,7 @@
         <v>1</v>
       </c>
       <c r="B191">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C191" t="b">
         <v>1</v>
@@ -2489,10 +2489,10 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192">
-        <v>550</v>
+        <v>700</v>
       </c>
       <c r="B192">
-        <v>271</v>
+        <v>2</v>
       </c>
       <c r="C192" t="b">
         <v>0</v>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="B193">
         <v>1</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194">
-        <v>800</v>
+        <v>1</v>
       </c>
       <c r="B194">
         <v>1</v>
@@ -2522,51 +2522,51 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195">
-        <v>1080</v>
+        <v>2000</v>
       </c>
       <c r="B195">
         <v>1</v>
       </c>
       <c r="C195" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196">
-        <v>420</v>
+        <v>1</v>
       </c>
       <c r="B196">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197">
-        <v>1</v>
+        <v>950</v>
       </c>
       <c r="B197">
         <v>1</v>
       </c>
       <c r="C197" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198">
-        <v>550</v>
+        <v>1400</v>
       </c>
       <c r="B198">
         <v>1</v>
       </c>
       <c r="C198" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199">
-        <v>650</v>
+        <v>750</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -2577,62 +2577,62 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200">
-        <v>550</v>
+        <v>1</v>
       </c>
       <c r="B200">
         <v>1</v>
       </c>
       <c r="C200" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201">
-        <v>1595</v>
+        <v>1200</v>
       </c>
       <c r="B201">
         <v>1</v>
       </c>
       <c r="C201" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="B202">
         <v>1</v>
       </c>
       <c r="C202" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203">
-        <v>765</v>
+        <v>1750</v>
       </c>
       <c r="B203">
         <v>1</v>
       </c>
       <c r="C203" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204">
-        <v>950</v>
+        <v>1</v>
       </c>
       <c r="B204">
         <v>1</v>
       </c>
       <c r="C204" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -2643,18 +2643,18 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206">
-        <v>1300</v>
+        <v>1</v>
       </c>
       <c r="B206">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="208" spans="1:3">
       <c r="A208">
-        <v>1</v>
+        <v>750</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -2676,10 +2676,10 @@
     </row>
     <row r="209" spans="1:3">
       <c r="A209">
-        <v>2000</v>
+        <v>825</v>
       </c>
       <c r="B209">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C209" t="b">
         <v>1</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="210" spans="1:3">
       <c r="A210">
-        <v>1</v>
+        <v>850</v>
       </c>
       <c r="B210">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C210" t="b">
         <v>1</v>
@@ -2698,18 +2698,18 @@
     </row>
     <row r="211" spans="1:3">
       <c r="A211">
-        <v>850</v>
+        <v>1</v>
       </c>
       <c r="B211">
         <v>1</v>
       </c>
       <c r="C211" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212">
-        <v>750</v>
+        <v>1</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -2720,13 +2720,13 @@
     </row>
     <row r="213" spans="1:3">
       <c r="A213">
-        <v>1000</v>
+        <v>2400</v>
       </c>
       <c r="B213">
         <v>1</v>
       </c>
       <c r="C213" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -2742,21 +2742,21 @@
     </row>
     <row r="215" spans="1:3">
       <c r="A215">
-        <v>575</v>
+        <v>1</v>
       </c>
       <c r="B215">
         <v>1</v>
       </c>
       <c r="C215" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="B216">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C216" t="b">
         <v>1</v>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="217" spans="1:3">
       <c r="A217">
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="B217">
         <v>1</v>
@@ -2775,106 +2775,106 @@
     </row>
     <row r="218" spans="1:3">
       <c r="A218">
-        <v>650</v>
+        <v>900</v>
       </c>
       <c r="B218">
         <v>1</v>
       </c>
       <c r="C218" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="B219">
         <v>1</v>
       </c>
       <c r="C219" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220">
-        <v>1</v>
+        <v>750</v>
       </c>
       <c r="B220">
         <v>1</v>
       </c>
       <c r="C220" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221">
-        <v>999</v>
+        <v>2400</v>
       </c>
       <c r="B221">
         <v>1</v>
       </c>
       <c r="C221" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222">
-        <v>1200</v>
+        <v>1</v>
       </c>
       <c r="B222">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C222" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="B223">
         <v>1</v>
       </c>
       <c r="C223" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224">
-        <v>800</v>
+        <v>2600</v>
       </c>
       <c r="B224">
         <v>1</v>
       </c>
       <c r="C224" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225">
-        <v>1</v>
+        <v>1250</v>
       </c>
       <c r="B225">
         <v>1</v>
       </c>
       <c r="C225" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="B226">
         <v>1</v>
       </c>
       <c r="C226" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227">
-        <v>1</v>
+        <v>1250</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -2885,1542 +2885,13 @@
     </row>
     <row r="228" spans="1:3">
       <c r="A228">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="B228">
         <v>1</v>
       </c>
       <c r="C228" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229">
-        <v>0</v>
-      </c>
-      <c r="B229">
-        <v>1</v>
-      </c>
-      <c r="C229" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3">
-      <c r="A230">
-        <v>700</v>
-      </c>
-      <c r="B230">
-        <v>1</v>
-      </c>
-      <c r="C230" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
-      <c r="A231">
-        <v>600</v>
-      </c>
-      <c r="B231">
-        <v>1</v>
-      </c>
-      <c r="C231" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3">
-      <c r="A232">
-        <v>1</v>
-      </c>
-      <c r="B232">
-        <v>1</v>
-      </c>
-      <c r="C232" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233">
-        <v>350</v>
-      </c>
-      <c r="B233">
-        <v>5</v>
-      </c>
-      <c r="C233" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3">
-      <c r="A234">
-        <v>400</v>
-      </c>
-      <c r="B234">
-        <v>1</v>
-      </c>
-      <c r="C234" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235">
-        <v>150</v>
-      </c>
-      <c r="B235">
-        <v>1</v>
-      </c>
-      <c r="C235" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
-      <c r="A236">
-        <v>650</v>
-      </c>
-      <c r="B236">
-        <v>1</v>
-      </c>
-      <c r="C236" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
-      <c r="A237">
-        <v>850</v>
-      </c>
-      <c r="B237">
-        <v>1</v>
-      </c>
-      <c r="C237" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
-      <c r="A238">
-        <v>550</v>
-      </c>
-      <c r="B238">
-        <v>6</v>
-      </c>
-      <c r="C238" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239">
-        <v>1950</v>
-      </c>
-      <c r="B239">
-        <v>1</v>
-      </c>
-      <c r="C239" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240">
-        <v>800</v>
-      </c>
-      <c r="B240">
-        <v>1</v>
-      </c>
-      <c r="C240" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3">
-      <c r="A241">
-        <v>925</v>
-      </c>
-      <c r="B241">
-        <v>1</v>
-      </c>
-      <c r="C241" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3">
-      <c r="A242">
-        <v>1168</v>
-      </c>
-      <c r="B242">
-        <v>1</v>
-      </c>
-      <c r="C242" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
-      <c r="A243">
-        <v>800</v>
-      </c>
-      <c r="B243">
-        <v>23</v>
-      </c>
-      <c r="C243" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="A244">
-        <v>1412</v>
-      </c>
-      <c r="B244">
-        <v>1</v>
-      </c>
-      <c r="C244" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3">
-      <c r="A245">
-        <v>1150</v>
-      </c>
-      <c r="B245">
-        <v>1</v>
-      </c>
-      <c r="C245" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3">
-      <c r="A246">
-        <v>600</v>
-      </c>
-      <c r="B246">
-        <v>1</v>
-      </c>
-      <c r="C246" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3">
-      <c r="A247">
-        <v>1200</v>
-      </c>
-      <c r="B247">
-        <v>1</v>
-      </c>
-      <c r="C247" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3">
-      <c r="A248">
-        <v>1</v>
-      </c>
-      <c r="B248">
-        <v>1</v>
-      </c>
-      <c r="C248" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
-      <c r="A249">
-        <v>2400</v>
-      </c>
-      <c r="B249">
-        <v>1</v>
-      </c>
-      <c r="C249" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3">
-      <c r="A250">
-        <v>1</v>
-      </c>
-      <c r="B250">
-        <v>1</v>
-      </c>
-      <c r="C250" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3">
-      <c r="A251">
-        <v>0</v>
-      </c>
-      <c r="B251">
-        <v>1</v>
-      </c>
-      <c r="C251" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
-      <c r="A252">
-        <v>600</v>
-      </c>
-      <c r="B252">
-        <v>1</v>
-      </c>
-      <c r="C252" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
-      <c r="A253">
-        <v>1</v>
-      </c>
-      <c r="B253">
-        <v>1</v>
-      </c>
-      <c r="C253" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
-      <c r="A254">
-        <v>700</v>
-      </c>
-      <c r="B254">
-        <v>1</v>
-      </c>
-      <c r="C254" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="A255">
-        <v>1</v>
-      </c>
-      <c r="B255">
-        <v>1</v>
-      </c>
-      <c r="C255" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3">
-      <c r="A256">
-        <v>700</v>
-      </c>
-      <c r="B256">
-        <v>1</v>
-      </c>
-      <c r="C256" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3">
-      <c r="A257">
-        <v>1</v>
-      </c>
-      <c r="B257">
-        <v>1</v>
-      </c>
-      <c r="C257" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
-      <c r="A258">
-        <v>1400</v>
-      </c>
-      <c r="B258">
-        <v>2</v>
-      </c>
-      <c r="C258" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="A259">
-        <v>900</v>
-      </c>
-      <c r="B259">
-        <v>1</v>
-      </c>
-      <c r="C259" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3">
-      <c r="A260">
-        <v>1000</v>
-      </c>
-      <c r="B260">
-        <v>1</v>
-      </c>
-      <c r="C260" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
-      <c r="A261">
-        <v>1</v>
-      </c>
-      <c r="B261">
-        <v>1</v>
-      </c>
-      <c r="C261" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3">
-      <c r="A262">
-        <v>1200</v>
-      </c>
-      <c r="B262">
-        <v>1</v>
-      </c>
-      <c r="C262" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3">
-      <c r="A263">
-        <v>950</v>
-      </c>
-      <c r="B263">
-        <v>1</v>
-      </c>
-      <c r="C263" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3">
-      <c r="A264">
-        <v>700</v>
-      </c>
-      <c r="B264">
-        <v>1</v>
-      </c>
-      <c r="C264" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3">
-      <c r="A265">
-        <v>879</v>
-      </c>
-      <c r="B265">
-        <v>2</v>
-      </c>
-      <c r="C265" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3">
-      <c r="A266">
-        <v>800</v>
-      </c>
-      <c r="B266">
-        <v>1</v>
-      </c>
-      <c r="C266" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3">
-      <c r="A267">
-        <v>795</v>
-      </c>
-      <c r="B267">
-        <v>1</v>
-      </c>
-      <c r="C267" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3">
-      <c r="A268">
-        <v>500</v>
-      </c>
-      <c r="B268">
-        <v>4</v>
-      </c>
-      <c r="C268" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3">
-      <c r="A269">
-        <v>300</v>
-      </c>
-      <c r="B269">
-        <v>5</v>
-      </c>
-      <c r="C269" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3">
-      <c r="A270">
-        <v>1050</v>
-      </c>
-      <c r="B270">
-        <v>2</v>
-      </c>
-      <c r="C270" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3">
-      <c r="A271">
-        <v>1</v>
-      </c>
-      <c r="B271">
-        <v>1</v>
-      </c>
-      <c r="C271" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3">
-      <c r="A272">
-        <v>1</v>
-      </c>
-      <c r="B272">
-        <v>1</v>
-      </c>
-      <c r="C272" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3">
-      <c r="A273">
-        <v>1750</v>
-      </c>
-      <c r="B273">
-        <v>1</v>
-      </c>
-      <c r="C273" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3">
-      <c r="A274">
-        <v>700</v>
-      </c>
-      <c r="B274">
-        <v>2</v>
-      </c>
-      <c r="C274" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3">
-      <c r="A275">
-        <v>950</v>
-      </c>
-      <c r="B275">
-        <v>1</v>
-      </c>
-      <c r="C275" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3">
-      <c r="A276">
-        <v>650</v>
-      </c>
-      <c r="B276">
-        <v>1</v>
-      </c>
-      <c r="C276" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3">
-      <c r="A277">
-        <v>999</v>
-      </c>
-      <c r="B277">
-        <v>1</v>
-      </c>
-      <c r="C277" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3">
-      <c r="A278">
-        <v>1</v>
-      </c>
-      <c r="B278">
-        <v>1</v>
-      </c>
-      <c r="C278" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3">
-      <c r="A279">
-        <v>1</v>
-      </c>
-      <c r="B279">
-        <v>1</v>
-      </c>
-      <c r="C279" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3">
-      <c r="A280">
-        <v>1</v>
-      </c>
-      <c r="B280">
-        <v>1</v>
-      </c>
-      <c r="C280" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3">
-      <c r="A281">
-        <v>2500</v>
-      </c>
-      <c r="B281">
-        <v>1</v>
-      </c>
-      <c r="C281" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3">
-      <c r="A282">
-        <v>800</v>
-      </c>
-      <c r="B282">
-        <v>1</v>
-      </c>
-      <c r="C282" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3">
-      <c r="A283">
-        <v>900</v>
-      </c>
-      <c r="B283">
-        <v>12</v>
-      </c>
-      <c r="C283" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3">
-      <c r="A284">
-        <v>1200</v>
-      </c>
-      <c r="B284">
-        <v>2</v>
-      </c>
-      <c r="C284" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3">
-      <c r="A285">
-        <v>1</v>
-      </c>
-      <c r="B285">
-        <v>1</v>
-      </c>
-      <c r="C285" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3">
-      <c r="A286">
-        <v>1</v>
-      </c>
-      <c r="B286">
-        <v>1</v>
-      </c>
-      <c r="C286" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3">
-      <c r="A287">
-        <v>800</v>
-      </c>
-      <c r="B287">
-        <v>1</v>
-      </c>
-      <c r="C287" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3">
-      <c r="A288">
-        <v>1</v>
-      </c>
-      <c r="B288">
-        <v>1</v>
-      </c>
-      <c r="C288" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3">
-      <c r="A289">
-        <v>1</v>
-      </c>
-      <c r="B289">
-        <v>1</v>
-      </c>
-      <c r="C289" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3">
-      <c r="A290">
-        <v>1</v>
-      </c>
-      <c r="B290">
-        <v>1</v>
-      </c>
-      <c r="C290" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3">
-      <c r="A291">
-        <v>300</v>
-      </c>
-      <c r="B291">
-        <v>1</v>
-      </c>
-      <c r="C291" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3">
-      <c r="A292">
-        <v>1</v>
-      </c>
-      <c r="B292">
-        <v>1</v>
-      </c>
-      <c r="C292" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3">
-      <c r="A293">
-        <v>800</v>
-      </c>
-      <c r="B293">
-        <v>1</v>
-      </c>
-      <c r="C293" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3">
-      <c r="A294">
-        <v>1</v>
-      </c>
-      <c r="B294">
-        <v>1</v>
-      </c>
-      <c r="C294" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3">
-      <c r="A295">
-        <v>800</v>
-      </c>
-      <c r="B295">
-        <v>1</v>
-      </c>
-      <c r="C295" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3">
-      <c r="A296">
-        <v>1000</v>
-      </c>
-      <c r="B296">
-        <v>2</v>
-      </c>
-      <c r="C296" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3">
-      <c r="A297">
-        <v>1</v>
-      </c>
-      <c r="B297">
-        <v>1</v>
-      </c>
-      <c r="C297" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3">
-      <c r="A298">
-        <v>1</v>
-      </c>
-      <c r="B298">
-        <v>1</v>
-      </c>
-      <c r="C298" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3">
-      <c r="A299">
-        <v>1</v>
-      </c>
-      <c r="B299">
-        <v>1</v>
-      </c>
-      <c r="C299" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3">
-      <c r="A300">
-        <v>2000</v>
-      </c>
-      <c r="B300">
-        <v>1</v>
-      </c>
-      <c r="C300" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3">
-      <c r="A301">
-        <v>375</v>
-      </c>
-      <c r="B301">
-        <v>1</v>
-      </c>
-      <c r="C301" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3">
-      <c r="A302">
-        <v>650</v>
-      </c>
-      <c r="B302">
-        <v>1</v>
-      </c>
-      <c r="C302" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3">
-      <c r="A303">
-        <v>1</v>
-      </c>
-      <c r="B303">
-        <v>1</v>
-      </c>
-      <c r="C303" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3">
-      <c r="A304">
-        <v>1200</v>
-      </c>
-      <c r="B304">
-        <v>1</v>
-      </c>
-      <c r="C304" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3">
-      <c r="A305">
-        <v>750</v>
-      </c>
-      <c r="B305">
-        <v>1</v>
-      </c>
-      <c r="C305" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3">
-      <c r="A306">
-        <v>1</v>
-      </c>
-      <c r="B306">
-        <v>1</v>
-      </c>
-      <c r="C306" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3">
-      <c r="A307">
-        <v>825</v>
-      </c>
-      <c r="B307">
-        <v>4</v>
-      </c>
-      <c r="C307" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3">
-      <c r="A308">
-        <v>700</v>
-      </c>
-      <c r="B308">
-        <v>2</v>
-      </c>
-      <c r="C308" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3">
-      <c r="A309">
-        <v>1000</v>
-      </c>
-      <c r="B309">
-        <v>2</v>
-      </c>
-      <c r="C309" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3">
-      <c r="A310">
-        <v>850</v>
-      </c>
-      <c r="B310">
-        <v>1</v>
-      </c>
-      <c r="C310" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3">
-      <c r="A311">
-        <v>300</v>
-      </c>
-      <c r="B311">
-        <v>1</v>
-      </c>
-      <c r="C311" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3">
-      <c r="A312">
-        <v>850</v>
-      </c>
-      <c r="B312">
-        <v>2</v>
-      </c>
-      <c r="C312" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3">
-      <c r="A313">
-        <v>1</v>
-      </c>
-      <c r="B313">
-        <v>2</v>
-      </c>
-      <c r="C313" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3">
-      <c r="A314">
-        <v>800</v>
-      </c>
-      <c r="B314">
-        <v>1</v>
-      </c>
-      <c r="C314" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3">
-      <c r="A315">
-        <v>1</v>
-      </c>
-      <c r="B315">
-        <v>1</v>
-      </c>
-      <c r="C315" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3">
-      <c r="A316">
-        <v>1</v>
-      </c>
-      <c r="B316">
-        <v>1</v>
-      </c>
-      <c r="C316" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3">
-      <c r="A317">
-        <v>1</v>
-      </c>
-      <c r="B317">
-        <v>1</v>
-      </c>
-      <c r="C317" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="318" spans="1:3">
-      <c r="A318">
-        <v>750</v>
-      </c>
-      <c r="B318">
-        <v>1</v>
-      </c>
-      <c r="C318" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3">
-      <c r="A319">
-        <v>800</v>
-      </c>
-      <c r="B319">
-        <v>1</v>
-      </c>
-      <c r="C319" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="320" spans="1:3">
-      <c r="A320">
-        <v>800</v>
-      </c>
-      <c r="B320">
-        <v>1</v>
-      </c>
-      <c r="C320" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="321" spans="1:3">
-      <c r="A321">
-        <v>1400</v>
-      </c>
-      <c r="B321">
-        <v>1</v>
-      </c>
-      <c r="C321" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="322" spans="1:3">
-      <c r="A322">
-        <v>600</v>
-      </c>
-      <c r="B322">
-        <v>1</v>
-      </c>
-      <c r="C322" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3">
-      <c r="A323">
-        <v>1</v>
-      </c>
-      <c r="B323">
-        <v>1</v>
-      </c>
-      <c r="C323" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3">
-      <c r="A324">
-        <v>123456</v>
-      </c>
-      <c r="B324">
-        <v>1</v>
-      </c>
-      <c r="C324" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3">
-      <c r="A325">
-        <v>1</v>
-      </c>
-      <c r="B325">
-        <v>1</v>
-      </c>
-      <c r="C325" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3">
-      <c r="A326">
-        <v>750</v>
-      </c>
-      <c r="B326">
-        <v>1</v>
-      </c>
-      <c r="C326" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="327" spans="1:3">
-      <c r="A327">
-        <v>1000</v>
-      </c>
-      <c r="B327">
-        <v>1</v>
-      </c>
-      <c r="C327" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="328" spans="1:3">
-      <c r="A328">
-        <v>800</v>
-      </c>
-      <c r="B328">
-        <v>1</v>
-      </c>
-      <c r="C328" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3">
-      <c r="A329">
-        <v>2000</v>
-      </c>
-      <c r="B329">
-        <v>1</v>
-      </c>
-      <c r="C329" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3">
-      <c r="A330">
-        <v>1</v>
-      </c>
-      <c r="B330">
-        <v>2</v>
-      </c>
-      <c r="C330" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="331" spans="1:3">
-      <c r="A331">
-        <v>800</v>
-      </c>
-      <c r="B331">
-        <v>1</v>
-      </c>
-      <c r="C331" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="332" spans="1:3">
-      <c r="A332">
-        <v>800</v>
-      </c>
-      <c r="B332">
-        <v>1</v>
-      </c>
-      <c r="C332" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="333" spans="1:3">
-      <c r="A333">
-        <v>800</v>
-      </c>
-      <c r="B333">
-        <v>4</v>
-      </c>
-      <c r="C333" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="334" spans="1:3">
-      <c r="A334">
-        <v>1</v>
-      </c>
-      <c r="B334">
-        <v>1</v>
-      </c>
-      <c r="C334" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="335" spans="1:3">
-      <c r="A335">
-        <v>800</v>
-      </c>
-      <c r="B335">
-        <v>1</v>
-      </c>
-      <c r="C335" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3">
-      <c r="A336">
-        <v>1</v>
-      </c>
-      <c r="B336">
-        <v>1</v>
-      </c>
-      <c r="C336" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="337" spans="1:3">
-      <c r="A337">
-        <v>1</v>
-      </c>
-      <c r="B337">
-        <v>1</v>
-      </c>
-      <c r="C337" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="338" spans="1:3">
-      <c r="A338">
-        <v>1300</v>
-      </c>
-      <c r="B338">
-        <v>1</v>
-      </c>
-      <c r="C338" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="339" spans="1:3">
-      <c r="A339">
-        <v>1</v>
-      </c>
-      <c r="B339">
-        <v>1</v>
-      </c>
-      <c r="C339" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="340" spans="1:3">
-      <c r="A340">
-        <v>800</v>
-      </c>
-      <c r="B340">
-        <v>5</v>
-      </c>
-      <c r="C340" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="341" spans="1:3">
-      <c r="A341">
-        <v>800</v>
-      </c>
-      <c r="B341">
-        <v>1</v>
-      </c>
-      <c r="C341" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="342" spans="1:3">
-      <c r="A342">
-        <v>1</v>
-      </c>
-      <c r="B342">
-        <v>2</v>
-      </c>
-      <c r="C342" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3">
-      <c r="A343">
-        <v>1</v>
-      </c>
-      <c r="B343">
-        <v>1</v>
-      </c>
-      <c r="C343" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="344" spans="1:3">
-      <c r="A344">
-        <v>500</v>
-      </c>
-      <c r="B344">
-        <v>1</v>
-      </c>
-      <c r="C344" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3">
-      <c r="A345">
-        <v>750</v>
-      </c>
-      <c r="B345">
-        <v>1</v>
-      </c>
-      <c r="C345" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3">
-      <c r="A346">
-        <v>1</v>
-      </c>
-      <c r="B346">
-        <v>1</v>
-      </c>
-      <c r="C346" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3">
-      <c r="A347">
-        <v>0</v>
-      </c>
-      <c r="B347">
-        <v>1</v>
-      </c>
-      <c r="C347" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="348" spans="1:3">
-      <c r="A348">
-        <v>1</v>
-      </c>
-      <c r="B348">
-        <v>1</v>
-      </c>
-      <c r="C348" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="349" spans="1:3">
-      <c r="A349">
-        <v>1000</v>
-      </c>
-      <c r="B349">
-        <v>1</v>
-      </c>
-      <c r="C349" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="350" spans="1:3">
-      <c r="A350">
-        <v>900</v>
-      </c>
-      <c r="B350">
-        <v>1</v>
-      </c>
-      <c r="C350" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="351" spans="1:3">
-      <c r="A351">
-        <v>0</v>
-      </c>
-      <c r="B351">
-        <v>1</v>
-      </c>
-      <c r="C351" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="352" spans="1:3">
-      <c r="A352">
-        <v>0</v>
-      </c>
-      <c r="B352">
-        <v>1</v>
-      </c>
-      <c r="C352" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="353" spans="1:3">
-      <c r="A353">
-        <v>1000</v>
-      </c>
-      <c r="B353">
-        <v>2</v>
-      </c>
-      <c r="C353" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="354" spans="1:3">
-      <c r="A354">
-        <v>1200</v>
-      </c>
-      <c r="B354">
-        <v>2</v>
-      </c>
-      <c r="C354" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="355" spans="1:3">
-      <c r="A355">
-        <v>700</v>
-      </c>
-      <c r="B355">
-        <v>1</v>
-      </c>
-      <c r="C355" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="356" spans="1:3">
-      <c r="A356">
-        <v>500</v>
-      </c>
-      <c r="B356">
-        <v>1</v>
-      </c>
-      <c r="C356" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="357" spans="1:3">
-      <c r="A357">
-        <v>1</v>
-      </c>
-      <c r="B357">
-        <v>1</v>
-      </c>
-      <c r="C357" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="358" spans="1:3">
-      <c r="A358">
-        <v>1</v>
-      </c>
-      <c r="B358">
-        <v>1</v>
-      </c>
-      <c r="C358" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="359" spans="1:3">
-      <c r="A359">
-        <v>1</v>
-      </c>
-      <c r="B359">
-        <v>1</v>
-      </c>
-      <c r="C359" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="360" spans="1:3">
-      <c r="A360">
-        <v>700</v>
-      </c>
-      <c r="B360">
-        <v>1</v>
-      </c>
-      <c r="C360" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="361" spans="1:3">
-      <c r="A361">
-        <v>0</v>
-      </c>
-      <c r="B361">
-        <v>1</v>
-      </c>
-      <c r="C361" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="362" spans="1:3">
-      <c r="A362">
-        <v>1</v>
-      </c>
-      <c r="B362">
-        <v>1</v>
-      </c>
-      <c r="C362" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="363" spans="1:3">
-      <c r="A363">
-        <v>0</v>
-      </c>
-      <c r="B363">
-        <v>2</v>
-      </c>
-      <c r="C363" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="364" spans="1:3">
-      <c r="A364">
-        <v>0</v>
-      </c>
-      <c r="B364">
-        <v>2</v>
-      </c>
-      <c r="C364" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="365" spans="1:3">
-      <c r="A365">
-        <v>0</v>
-      </c>
-      <c r="B365">
-        <v>1</v>
-      </c>
-      <c r="C365" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="366" spans="1:3">
-      <c r="A366">
-        <v>1</v>
-      </c>
-      <c r="B366">
-        <v>1</v>
-      </c>
-      <c r="C366" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="367" spans="1:3">
-      <c r="A367">
-        <v>1</v>
-      </c>
-      <c r="B367">
-        <v>1</v>
-      </c>
-      <c r="C367" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>